<commit_message>
Fixed name of matlab package
</commit_message>
<xml_diff>
--- a/figures/tables.xlsx
+++ b/figures/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stewart\Documents\2019spring\CS760_project\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEBECCA5-5692-4891-8134-3DEB00CF1F2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7376B53-D8E2-4DA6-8AB7-0771A59EB038}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E26474BE-6514-43A6-B442-AD29B3FF278F}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>bnstruct</t>
   </si>
   <si>
-    <t>BNT</t>
-  </si>
-  <si>
     <t>Precision</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Time steps</t>
+  </si>
+  <si>
+    <t>Global MIT</t>
   </si>
 </sst>
 </file>
@@ -449,12 +449,12 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
@@ -468,16 +468,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added the newest arabidopsis results
</commit_message>
<xml_diff>
--- a/figures/tables.xlsx
+++ b/figures/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stewart\Documents\2019spring\CS760_project\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7376B53-D8E2-4DA6-8AB7-0771A59EB038}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0A6C1C-ED06-4F70-B243-CF15D025EDEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E26474BE-6514-43A6-B442-AD29B3FF278F}"/>
+    <workbookView xWindow="5760" yWindow="3336" windowWidth="17280" windowHeight="9024" xr2:uid="{E26474BE-6514-43A6-B442-AD29B3FF278F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Dataset</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>Global MIT</t>
+  </si>
+  <si>
+    <t>bnstruct, arabidopsis, 3, 0.533, 0.475, 0.368</t>
+  </si>
+  <si>
+    <t>bnstruct, arabidopsis, 4, 0.491, 0.436, 0.451</t>
+  </si>
+  <si>
+    <t>bnstruct, arabidopsis, 5, 0.512, 0.458, 0.469</t>
+  </si>
+  <si>
+    <t>bnstruct, arabidopsis, 6, 0.472, 0.425, 0.497</t>
+  </si>
+  <si>
+    <t>bnstruct, arabidopsis, 7, 0.573, 0.577, 0.189</t>
+  </si>
+  <si>
+    <t>bnstruct, arabidopsis, 8, 0.557, 0.532, 0.136</t>
   </si>
 </sst>
 </file>
@@ -73,7 +91,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +109,12 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -124,13 +148,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0531A08A-963C-4AA8-A9D2-B71E21D41DCA}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A12" sqref="A12:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -602,22 +629,92 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.36799999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.45100000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D10" s="1">
         <v>0.54500000000000004</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E10" s="3">
         <v>0.77</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F10" s="3">
         <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>